<commit_message>
UU beats ZZ on relative preferred mentor rank
</commit_message>
<xml_diff>
--- a/tests/files/mentormatch_example_applications.xlsx
+++ b/tests/files/mentormatch_example_applications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\mentormatch\tests\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A35912-6E99-4162-8683-470F362238CB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DCA7EA-F067-4918-A5AB-4F2345300B26}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentors" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="163">
   <si>
     <t>ID</t>
   </si>
@@ -215,9 +215,6 @@
   </si>
   <si>
     <t>Malvern</t>
-  </si>
-  <si>
-    <t>10</t>
   </si>
   <si>
     <t>5.5</t>
@@ -1167,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,7 +1299,7 @@
         <v>26</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>35</v>
@@ -1350,13 +1347,13 @@
         <v>47</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC2" s="3" t="s">
         <v>49</v>
@@ -1406,21 +1403,21 @@
       <c r="N3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="2">
+        <v>20</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="S3" s="3"/>
       <c r="T3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U3" s="3" t="s">
         <v>46</v>
@@ -1438,7 +1435,7 @@
         <v>45</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA3" s="3" t="s">
         <v>46</v>
@@ -1450,7 +1447,7 @@
         <v>49</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -1470,43 +1467,43 @@
         <v>31</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
@@ -1556,47 +1553,47 @@
         <v>31</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>55</v>
       </c>
       <c r="M5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="S5" s="3"/>
       <c r="T5" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U5" s="3" t="s">
         <v>46</v>
@@ -1614,7 +1611,7 @@
         <v>46</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AA5" s="3" t="s">
         <v>45</v>
@@ -1644,47 +1641,47 @@
         <v>31</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q6" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U6" s="3" t="s">
         <v>45</v>
@@ -1728,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D1D5B0-6A85-4C9E-B6D1-7EF108D8DFB6}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,9 +1735,14 @@
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.5703125" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="14" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" customWidth="1"/>
+    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="7" customWidth="1"/>
-    <col min="17" max="17" width="8.5703125" customWidth="1"/>
+    <col min="17" max="17" width="19.140625" customWidth="1"/>
     <col min="18" max="18" width="8.85546875" customWidth="1"/>
     <col min="19" max="19" width="29" bestFit="1" customWidth="1"/>
     <col min="20" max="31" width="20" bestFit="1" customWidth="1"/>
@@ -1799,13 +1801,13 @@
         <v>16</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>20</v>
@@ -1823,7 +1825,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>26</v>
@@ -1832,7 +1834,7 @@
         <v>27</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>28</v>
@@ -1858,49 +1860,49 @@
         <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="N2" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>49</v>
       </c>
       <c r="S2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>45</v>
@@ -1927,13 +1929,13 @@
         <v>46</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>49</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -1953,47 +1955,47 @@
         <v>31</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>57</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>49</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
@@ -2026,38 +2028,38 @@
         <v>31</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="P4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>47</v>
@@ -2089,7 +2091,7 @@
         <v>47</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AD4" s="3" t="s">
         <v>49</v>
@@ -2113,38 +2115,38 @@
         <v>31</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="P5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>47</v>
@@ -2176,7 +2178,7 @@
         <v>45</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AD5" s="3" t="s">
         <v>49</v>
@@ -2200,28 +2202,28 @@
         <v>31</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>38</v>
@@ -2230,7 +2232,7 @@
         <v>39</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>41</v>
@@ -2265,7 +2267,7 @@
         <v>45</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD6" s="3" t="s">
         <v>49</v>
@@ -2279,47 +2281,47 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J7" s="3">
         <v>432198765</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="N7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>49</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U7" s="3" t="s">
         <v>45</v>
@@ -2346,13 +2348,13 @@
         <v>46</v>
       </c>
       <c r="AC7" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AD7" s="3" t="s">
         <v>49</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2372,7 +2374,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,10 +2384,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" t="s">
         <v>157</v>
-      </c>
-      <c r="B1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2393,7 +2395,7 @@
         <v>876543219</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2401,7 +2403,7 @@
         <v>654321987</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2421,17 +2423,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>